<commit_message>
added welcome with personalized msg
</commit_message>
<xml_diff>
--- a/facultymembers.xlsx
+++ b/facultymembers.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>Finance</t>
+  </si>
+  <si>
+    <t>Ruwayd</t>
+  </si>
+  <si>
+    <t>ESC</t>
+  </si>
+  <si>
+    <t>rmushtaq</t>
+  </si>
+  <si>
+    <t>Compuet</t>
   </si>
 </sst>
 </file>
@@ -104,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -178,6 +190,23 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
allot of update i forgor
</commit_message>
<xml_diff>
--- a/facultymembers.xlsx
+++ b/facultymembers.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -29,64 +29,55 @@
     <t>Research Interest</t>
   </si>
   <si>
-    <t>Talha</t>
-  </si>
-  <si>
-    <t>Ecology</t>
-  </si>
-  <si>
-    <t>talha@uoguelph</t>
-  </si>
-  <si>
-    <t>UC</t>
-  </si>
-  <si>
-    <t>biology</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>travis</t>
-  </si>
-  <si>
-    <t>scott</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>qs</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>Raahim</t>
-  </si>
-  <si>
-    <t>Engineering</t>
-  </si>
-  <si>
-    <t>rham@uoguelph.ca</t>
-  </si>
-  <si>
-    <t>ROZH Washroom</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>Ruwayd</t>
-  </si>
-  <si>
-    <t>ESC</t>
-  </si>
-  <si>
-    <t>rmushtaq</t>
-  </si>
-  <si>
-    <t>Compuet</t>
+    <t>Alan Turing</t>
+  </si>
+  <si>
+    <t>PH.D.</t>
+  </si>
+  <si>
+    <t>turing@university.edu</t>
+  </si>
+  <si>
+    <t>Room 201</t>
+  </si>
+  <si>
+    <t>Computational Theory</t>
+  </si>
+  <si>
+    <t>Emily Brontë</t>
+  </si>
+  <si>
+    <t>Master's</t>
+  </si>
+  <si>
+    <t>bronte@university.edu</t>
+  </si>
+  <si>
+    <t>Room 202</t>
+  </si>
+  <si>
+    <t>English Literature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grace Hopper </t>
+  </si>
+  <si>
+    <t>PHD</t>
+  </si>
+  <si>
+    <t>hopper@university.edu</t>
+  </si>
+  <si>
+    <t>Lab 203</t>
+  </si>
+  <si>
+    <t>Computer Programming</t>
+  </si>
+  <si>
+    <t>Lakyn Copeland</t>
+  </si>
+  <si>
+    <t>copeland@university.edu</t>
   </si>
 </sst>
 </file>
@@ -131,7 +122,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -176,67 +167,50 @@
         <v>10</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>